<commit_message>
cas-19 fixed flattening issue with pandas_excel_reader
</commit_message>
<xml_diff>
--- a/tests/tests_pandas_excel/good_sheet.xlsx
+++ b/tests/tests_pandas_excel/good_sheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zacharywolpov/casie/llama-hub/tests/tests_confluence/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zacharywolpov/casie/llama-hub/tests/tests_pandas_excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D86F37D5-EDCF-9C42-9828-DC8A6F36BFB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A7741E1-4739-494F-9CF5-11002B4B9078}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{7C040F9B-C288-5349-BC39-CB5FEDD891D1}"/>
   </bookViews>
@@ -399,7 +399,7 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>